<commit_message>
db추가, main.do 부분 수정, csv 추가
</commit_message>
<xml_diff>
--- a/data/docs/csv/picture.xlsx
+++ b/data/docs/csv/picture.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KHRDI-05\Desktop\project_hotel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\workspace-jsp\project_hotel\data\docs\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="198">
   <si>
     <t>null</t>
   </si>
@@ -377,78 +377,6 @@
     <t>s_premier4.jpg</t>
   </si>
   <si>
-    <t>pacific1.jpg</t>
-  </si>
-  <si>
-    <t>pacific2.jpg</t>
-  </si>
-  <si>
-    <t>pacific3.jpg</t>
-  </si>
-  <si>
-    <t>pacific4.jpg</t>
-  </si>
-  <si>
-    <t>presidential1.jpg</t>
-  </si>
-  <si>
-    <t>presidential2.jpg</t>
-  </si>
-  <si>
-    <t>presidential3.jpg</t>
-  </si>
-  <si>
-    <t>presidential4.jpg</t>
-  </si>
-  <si>
-    <t>royal1.jpg</t>
-  </si>
-  <si>
-    <t>royal2.jpg</t>
-  </si>
-  <si>
-    <t>royal3.jpg</t>
-  </si>
-  <si>
-    <t>royal4.jpg</t>
-  </si>
-  <si>
-    <t>s_pacific1.jpg</t>
-  </si>
-  <si>
-    <t>s_pacific2.jpg</t>
-  </si>
-  <si>
-    <t>s_pacific3.jpg</t>
-  </si>
-  <si>
-    <t>s_pacific4.jpg</t>
-  </si>
-  <si>
-    <t>s_presidential1.jpg</t>
-  </si>
-  <si>
-    <t>s_presidential2.jpg</t>
-  </si>
-  <si>
-    <t>s_presidential3.jpg</t>
-  </si>
-  <si>
-    <t>s_presidential4.jpg</t>
-  </si>
-  <si>
-    <t>s_royal1.jpg</t>
-  </si>
-  <si>
-    <t>s_royal2.jpg</t>
-  </si>
-  <si>
-    <t>s_royal3.jpg</t>
-  </si>
-  <si>
-    <t>s_royal4.jpg</t>
-  </si>
-  <si>
     <t>activity1.jpg</t>
   </si>
   <si>
@@ -594,6 +522,106 @@
   </si>
   <si>
     <t>s_activity12.jpg</t>
+  </si>
+  <si>
+    <t>pacific_deluxe1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pacific_deluxe2.jpg</t>
+  </si>
+  <si>
+    <t>pacific_deluxe3.jpg</t>
+  </si>
+  <si>
+    <t>pacific_deluxe4.jpg</t>
+  </si>
+  <si>
+    <t>presidential_suite1.jpg</t>
+  </si>
+  <si>
+    <t>presidential_suite2.jpg</t>
+  </si>
+  <si>
+    <t>presidential_suite3.jpg</t>
+  </si>
+  <si>
+    <t>presidential_suite4.jpg</t>
+  </si>
+  <si>
+    <t>royal_suite1.jpg</t>
+  </si>
+  <si>
+    <t>royal_suite2.jpg</t>
+  </si>
+  <si>
+    <t>royal_suite3.jpg</t>
+  </si>
+  <si>
+    <t>royal_suite4.jpg</t>
+  </si>
+  <si>
+    <t>s_pacific_deluxe1.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s_pacific_deluxe2.jpg</t>
+  </si>
+  <si>
+    <t>s_pacific_deluxe3.jpg</t>
+  </si>
+  <si>
+    <t>s_pacific_deluxe4.jpg</t>
+  </si>
+  <si>
+    <t>s_presidential_suite1.jpg</t>
+  </si>
+  <si>
+    <t>s_presidential_suite2.jpg</t>
+  </si>
+  <si>
+    <t>s_presidential_suite3.jpg</t>
+  </si>
+  <si>
+    <t>s_presidential_suite4.jpg</t>
+  </si>
+  <si>
+    <t>s_royal_suite1.jpg</t>
+  </si>
+  <si>
+    <t>s_royal_suite2.jpg</t>
+  </si>
+  <si>
+    <t>s_royal_suite3.jpg</t>
+  </si>
+  <si>
+    <t>s_royal_suite4.jpg</t>
+  </si>
+  <si>
+    <t>deluxe_content.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pacific_deluxe_content.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>premier_content.jpg</t>
+  </si>
+  <si>
+    <t>premier_terrace_content.jpg</t>
+  </si>
+  <si>
+    <t>presidential_suite_content.gif</t>
+  </si>
+  <si>
+    <t>royal_suite_content.gif</t>
+  </si>
+  <si>
+    <t>standard_content.jpg</t>
+  </si>
+  <si>
+    <t>terrace_content.jpg</t>
   </si>
 </sst>
 </file>
@@ -923,17 +951,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -949,227 +975,227 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1180,7 +1206,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1191,7 +1217,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1202,7 +1228,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1213,51 +1239,51 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1268,7 +1294,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1279,7 +1305,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1290,7 +1316,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1301,7 +1327,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1312,7 +1338,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1323,7 +1349,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1334,7 +1360,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1345,51 +1371,51 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1400,7 +1426,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1411,7 +1437,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1422,7 +1448,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -1433,51 +1459,51 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1488,7 +1514,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1499,7 +1525,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1510,7 +1536,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>177</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1521,51 +1547,51 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>187</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1576,7 +1602,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1587,7 +1613,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1598,7 +1624,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1609,54 +1635,54 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>0</v>
@@ -1664,10 +1690,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
@@ -1675,10 +1701,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
         <v>0</v>
@@ -1686,10 +1712,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
         <v>0</v>
@@ -1697,10 +1723,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
         <v>0</v>
@@ -1708,10 +1734,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" t="s">
         <v>0</v>
@@ -1719,10 +1745,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
         <v>0</v>
@@ -1730,10 +1756,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
         <v>0</v>
@@ -1741,10 +1767,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
         <v>0</v>
@@ -1752,10 +1778,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
         <v>0</v>
@@ -1763,10 +1789,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
         <v>0</v>
@@ -1774,10 +1800,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" t="s">
         <v>0</v>
@@ -1785,10 +1811,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
         <v>0</v>
@@ -1796,10 +1822,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
         <v>0</v>
@@ -1807,7 +1833,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -1818,7 +1844,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -1829,7 +1855,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -1840,7 +1866,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -1851,7 +1877,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -1862,7 +1888,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -1873,7 +1899,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -1884,7 +1910,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -1895,7 +1921,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -1906,7 +1932,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>69</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -1917,7 +1943,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>165</v>
+        <v>68</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -1928,7 +1954,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>67</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -1939,7 +1965,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>167</v>
+        <v>66</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -1950,7 +1976,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -1961,7 +1987,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -1972,10 +1998,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>170</v>
+        <v>63</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
@@ -1983,10 +2009,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="B96">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
@@ -1994,10 +2020,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>172</v>
+        <v>61</v>
       </c>
       <c r="B97">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
@@ -2005,10 +2031,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="B98">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C98" t="s">
         <v>0</v>
@@ -2016,10 +2042,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>59</v>
       </c>
       <c r="B99">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C99" t="s">
         <v>0</v>
@@ -2027,10 +2053,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>175</v>
+        <v>58</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
         <v>0</v>
@@ -2038,10 +2064,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C101" t="s">
         <v>0</v>
@@ -2049,10 +2075,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>
@@ -2060,7 +2086,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -2071,7 +2097,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -2082,7 +2108,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -2093,7 +2119,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -2104,7 +2130,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>182</v>
+        <v>122</v>
       </c>
       <c r="B107">
         <v>3</v>
@@ -2115,7 +2141,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>183</v>
+        <v>123</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -2126,7 +2152,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>184</v>
+        <v>124</v>
       </c>
       <c r="B109">
         <v>3</v>
@@ -2137,7 +2163,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -2148,7 +2174,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>186</v>
+        <v>126</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -2159,7 +2185,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>187</v>
+        <v>127</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -2170,7 +2196,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -2181,7 +2207,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -2192,7 +2218,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -2203,7 +2229,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -2214,10 +2240,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C117" t="s">
         <v>0</v>
@@ -2225,10 +2251,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="B118">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C118" t="s">
         <v>0</v>
@@ -2236,10 +2262,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="B119">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C119" t="s">
         <v>0</v>
@@ -2247,10 +2273,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="B120">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C120" t="s">
         <v>0</v>
@@ -2258,10 +2284,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C121" t="s">
         <v>0</v>
@@ -2269,10 +2295,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>66</v>
+        <v>160</v>
       </c>
       <c r="B122">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
@@ -2280,10 +2306,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
         <v>0</v>
@@ -2291,10 +2317,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C124" t="s">
         <v>0</v>
@@ -2302,10 +2328,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="B125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C125" t="s">
         <v>0</v>
@@ -2313,10 +2339,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C126" t="s">
         <v>0</v>
@@ -2324,10 +2350,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C127" t="s">
         <v>0</v>
@@ -2335,10 +2361,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B128">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
         <v>0</v>
@@ -2346,10 +2372,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C129" t="s">
         <v>0</v>
@@ -2357,10 +2383,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B130">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C130" t="s">
         <v>0</v>
@@ -2368,10 +2394,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C131" t="s">
         <v>0</v>
@@ -2379,10 +2405,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C132" t="s">
         <v>0</v>
@@ -2390,10 +2416,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C133" t="s">
         <v>0</v>
@@ -2401,10 +2427,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C134" t="s">
         <v>0</v>
@@ -2412,10 +2438,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B135">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C135" t="s">
         <v>0</v>
@@ -2423,10 +2449,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C136" t="s">
         <v>0</v>
@@ -2434,10 +2460,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B137">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C137" t="s">
         <v>0</v>
@@ -2445,10 +2471,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B138">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C138" t="s">
         <v>0</v>
@@ -2456,10 +2482,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B139">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139" t="s">
         <v>0</v>
@@ -2467,7 +2493,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B140">
         <v>4</v>
@@ -2478,7 +2504,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B141">
         <v>4</v>
@@ -2489,7 +2515,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B142">
         <v>4</v>
@@ -2500,7 +2526,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B143">
         <v>4</v>
@@ -2511,7 +2537,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B144">
         <v>4</v>
@@ -2522,7 +2548,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B145">
         <v>4</v>
@@ -2533,7 +2559,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B146">
         <v>4</v>
@@ -2544,7 +2570,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B147">
         <v>4</v>
@@ -2555,7 +2581,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B148">
         <v>4</v>
@@ -2566,7 +2592,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B149">
         <v>4</v>
@@ -2577,7 +2603,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B150">
         <v>4</v>
@@ -2588,7 +2614,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B151">
         <v>4</v>
@@ -2599,7 +2625,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B152">
         <v>4</v>
@@ -2610,7 +2636,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B153">
         <v>4</v>
@@ -2621,7 +2647,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B154">
         <v>4</v>
@@ -2632,7 +2658,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B155">
         <v>4</v>
@@ -2643,7 +2669,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B156">
         <v>4</v>
@@ -2654,7 +2680,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B157">
         <v>4</v>
@@ -2665,7 +2691,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B158">
         <v>4</v>
@@ -2676,7 +2702,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B159">
         <v>4</v>
@@ -2687,7 +2713,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B160">
         <v>4</v>
@@ -2698,7 +2724,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B161">
         <v>4</v>
@@ -2709,7 +2735,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B162">
         <v>4</v>
@@ -2720,7 +2746,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B163">
         <v>4</v>
@@ -2731,7 +2757,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B164">
         <v>4</v>
@@ -2742,7 +2768,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B165">
         <v>4</v>
@@ -2753,7 +2779,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B166">
         <v>4</v>
@@ -2764,7 +2790,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B167">
         <v>4</v>
@@ -2775,7 +2801,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B168">
         <v>4</v>
@@ -2786,7 +2812,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B169">
         <v>4</v>
@@ -2797,7 +2823,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B170">
         <v>4</v>
@@ -2808,7 +2834,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B171">
         <v>4</v>
@@ -2819,7 +2845,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B172">
         <v>4</v>
@@ -2830,7 +2856,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B173">
         <v>4</v>
@@ -2841,7 +2867,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B174">
         <v>4</v>
@@ -2852,7 +2878,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B175">
         <v>4</v>
@@ -2863,7 +2889,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B176">
         <v>4</v>
@@ -2874,7 +2900,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B177">
         <v>4</v>
@@ -2885,10 +2911,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
       <c r="B178">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C178" t="s">
         <v>0</v>
@@ -2896,10 +2922,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="B179">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C179" t="s">
         <v>0</v>
@@ -2907,10 +2933,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="B180">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C180" t="s">
         <v>0</v>
@@ -2918,10 +2944,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="B181">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C181" t="s">
         <v>0</v>
@@ -2929,10 +2955,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>6</v>
+        <v>150</v>
       </c>
       <c r="B182">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C182" t="s">
         <v>0</v>
@@ -2940,10 +2966,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>53</v>
+      </c>
+      <c r="B183">
         <v>5</v>
-      </c>
-      <c r="B183">
-        <v>4</v>
       </c>
       <c r="C183" t="s">
         <v>0</v>
@@ -2951,10 +2977,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B184">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C184" t="s">
         <v>0</v>
@@ -2962,10 +2988,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B185">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C185" t="s">
         <v>0</v>
@@ -2973,10 +2999,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B186">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
         <v>0</v>
@@ -2984,16 +3010,107 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="B187">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>196</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>190</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>197</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+      <c r="C190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>192</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>193</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>195</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>194</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="C195">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A188:C195">
+    <sortCondition ref="C188"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>